<commit_message>
ppt STS Java 2706
</commit_message>
<xml_diff>
--- a/03 Assessments/Trabalhos - Avaliação Final/Relação de Aluno 2022_1 Yduqs Desenv Software Java INTEGRADA.xlsx
+++ b/03 Assessments/Trabalhos - Avaliação Final/Relação de Aluno 2022_1 Yduqs Desenv Software Java INTEGRADA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\YduqsArea1\16 WydenArea1 Desenvolvimento de Software Java\03 Assessments\Trabalhos - Avaliação Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAACF725-10B6-4A3F-A2F4-7A84B6C31673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E09E157-B17E-4CD0-A2CF-DA87C4A98271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AB2021C7-8F1D-4AC7-BCF9-40C40499B57D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Alunos</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Trabalho fora do escopo; Título Incompatível do Trabalho; Sumário sem página</t>
   </si>
   <si>
-    <t>Trabalho fora do escopo;Título Incompatível do Trabalho; Sumário sem página</t>
-  </si>
-  <si>
     <t>BARBOSA, PAULO</t>
   </si>
   <si>
@@ -175,6 +172,12 @@
   </si>
   <si>
     <t>Murilo Carvalho de Freitas + 0,9</t>
+  </si>
+  <si>
+    <t>Trabalho fora do escopo;Título Incompatível do Trabalho; Sumário sem página; Numeração de pag errada 1. HMTL???; Refrências fora do padrão ABNT; Conclusão equivocada; Não descreveu implements/extends; Pag. 39 solta; Referencias Agile/Scrum????</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; CMMI; Site IDEAL; código 03 errado 30 alunos???. -0,5 pelo atraso (não descontei); </t>
   </si>
 </sst>
 </file>
@@ -389,11 +392,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,7 +714,7 @@
   <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,28 +757,28 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="18" t="s">
         <v>21</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>17</v>
       </c>
       <c r="Y5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="16.5" x14ac:dyDescent="0.3">
@@ -1169,7 +1172,7 @@
         <v>17</v>
       </c>
       <c r="Y7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="16.5" x14ac:dyDescent="0.3">
@@ -1247,7 +1250,7 @@
         <v>17</v>
       </c>
       <c r="Y8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="16.5" x14ac:dyDescent="0.3">
@@ -1411,7 +1414,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="9">
         <v>0.5</v>
@@ -1570,60 +1573,60 @@
         <v>33</v>
       </c>
       <c r="C13" s="9">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D13" s="9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G13" s="9">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="H13" s="9">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I13" s="9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="K13" s="9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="L13" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="M13" s="20">
-        <v>0</v>
-      </c>
-      <c r="N13" s="20">
-        <v>0</v>
-      </c>
-      <c r="O13" s="20">
-        <v>0</v>
-      </c>
-      <c r="P13" s="20">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="20">
-        <v>0</v>
-      </c>
-      <c r="R13" s="20">
-        <v>0</v>
-      </c>
-      <c r="S13" s="20">
-        <v>0</v>
-      </c>
-      <c r="T13" s="20">
-        <v>0</v>
-      </c>
-      <c r="U13" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="N13" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="O13" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="P13" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>0</v>
+      </c>
+      <c r="R13" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="S13" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="T13" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="U13" s="9">
         <v>0</v>
       </c>
       <c r="V13" s="20">
@@ -1631,7 +1634,7 @@
       </c>
       <c r="W13" s="16">
         <f t="shared" si="0"/>
-        <v>0.99999999999999989</v>
+        <v>6.3</v>
       </c>
       <c r="X13" s="16" t="s">
         <v>17</v>
@@ -1648,60 +1651,60 @@
         <v>34</v>
       </c>
       <c r="C14" s="9">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D14" s="9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F14" s="9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G14" s="9">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="H14" s="9">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I14" s="9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="K14" s="9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="L14" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="M14" s="20">
-        <v>0</v>
-      </c>
-      <c r="N14" s="20">
-        <v>0</v>
-      </c>
-      <c r="O14" s="20">
-        <v>0</v>
-      </c>
-      <c r="P14" s="20">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="20">
-        <v>0</v>
-      </c>
-      <c r="R14" s="20">
-        <v>0</v>
-      </c>
-      <c r="S14" s="20">
-        <v>0</v>
-      </c>
-      <c r="T14" s="20">
-        <v>0</v>
-      </c>
-      <c r="U14" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="M14" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="N14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="O14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="P14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>0</v>
+      </c>
+      <c r="R14" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="S14" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="T14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="U14" s="9">
         <v>0</v>
       </c>
       <c r="V14" s="20">
@@ -1709,13 +1712,13 @@
       </c>
       <c r="W14" s="16">
         <f t="shared" si="0"/>
-        <v>0.99999999999999989</v>
+        <v>6.3</v>
       </c>
       <c r="X14" s="16" t="s">
         <v>17</v>
       </c>
       <c r="Y14" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="16.5" x14ac:dyDescent="0.3">
@@ -1723,7 +1726,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="22">
         <v>0</v>
@@ -1790,13 +1793,16 @@
         <v>0</v>
       </c>
       <c r="X15" s="16"/>
+      <c r="Y15" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>13</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="22">
         <v>0</v>
@@ -1869,7 +1875,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="22">
         <v>0</v>
@@ -1942,7 +1948,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="22">
         <v>0</v>
@@ -2015,7 +2021,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="22">
         <v>0</v>
@@ -2087,8 +2093,8 @@
       <c r="A20" s="23">
         <v>17</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>41</v>
+      <c r="B20" s="24" t="s">
+        <v>40</v>
       </c>
       <c r="C20" s="22">
         <v>0</v>
@@ -2155,7 +2161,7 @@
         <v>0</v>
       </c>
       <c r="X20" s="16"/>
-      <c r="Y20" s="26">
+      <c r="Y20" s="25">
         <v>0.7</v>
       </c>
     </row>
@@ -2186,7 +2192,7 @@
     </row>
     <row r="22" spans="1:25" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>